<commit_message>
backend and frontend update on 18-12
</commit_message>
<xml_diff>
--- a/backend/uploads/currentinventory_1_uk_december2025.xlsx
+++ b/backend/uploads/currentinventory_1_uk_december2025.xlsx
@@ -565,25 +565,25 @@
         <v>28</v>
       </c>
       <c r="D2">
-        <v>5052</v>
+        <v>4906</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>5009</v>
+        <v>4862</v>
       </c>
       <c r="G2">
         <v>86</v>
       </c>
       <c r="H2">
-        <v>5009</v>
+        <v>4862</v>
       </c>
       <c r="I2" s="2">
-        <v>46001.46237803435</v>
+        <v>46009.22343447226</v>
       </c>
       <c r="J2">
-        <v>5076</v>
+        <v>4941</v>
       </c>
       <c r="K2">
         <v>220</v>
@@ -592,10 +592,10 @@
         <v>0</v>
       </c>
       <c r="M2">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="N2">
-        <v>5009</v>
+        <v>4862</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -609,25 +609,25 @@
         <v>29</v>
       </c>
       <c r="D3">
-        <v>912</v>
+        <v>893</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>862</v>
       </c>
       <c r="G3">
-        <v>1822</v>
+        <v>60</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>862</v>
       </c>
       <c r="I3" s="2">
-        <v>46001.46237803435</v>
+        <v>46009.22343448379</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>845</v>
       </c>
       <c r="K3">
         <v>14</v>
@@ -636,10 +636,10 @@
         <v>0</v>
       </c>
       <c r="M3">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>862</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -653,25 +653,25 @@
         <v>30</v>
       </c>
       <c r="D4">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>578</v>
+        <v>241</v>
       </c>
       <c r="G4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H4">
-        <v>578</v>
+        <v>241</v>
       </c>
       <c r="I4" s="2">
-        <v>46001.46237803435</v>
+        <v>46009.22343448379</v>
       </c>
       <c r="J4">
-        <v>580</v>
+        <v>243</v>
       </c>
       <c r="K4">
         <v>11</v>
@@ -683,7 +683,7 @@
         <v>9</v>
       </c>
       <c r="N4">
-        <v>578</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -697,25 +697,25 @@
         <v>31</v>
       </c>
       <c r="D5">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I5" s="2">
-        <v>46001.46237803435</v>
+        <v>46009.22343448379</v>
       </c>
       <c r="J5">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K5">
         <v>4</v>
@@ -727,7 +727,7 @@
         <v>1</v>
       </c>
       <c r="N5">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -741,25 +741,25 @@
         <v>32</v>
       </c>
       <c r="D6">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>295</v>
+        <v>273</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>295</v>
+        <v>273</v>
       </c>
       <c r="I6" s="2">
-        <v>46001.46237803435</v>
+        <v>46009.22343448379</v>
       </c>
       <c r="J6">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="K6">
         <v>8</v>
@@ -768,10 +768,10 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="N6">
-        <v>295</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -785,25 +785,25 @@
         <v>33</v>
       </c>
       <c r="D7">
-        <v>957</v>
+        <v>894</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <v>946</v>
+        <v>887</v>
       </c>
       <c r="G7">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H7">
-        <v>946</v>
+        <v>887</v>
       </c>
       <c r="I7" s="2">
-        <v>46001.46237803435</v>
+        <v>46009.22343448379</v>
       </c>
       <c r="J7">
-        <v>971</v>
+        <v>915</v>
       </c>
       <c r="K7">
         <v>52</v>
@@ -812,10 +812,10 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N7">
-        <v>946</v>
+        <v>887</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -829,25 +829,25 @@
         <v>34</v>
       </c>
       <c r="D8">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
       <c r="H8">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="I8" s="2">
-        <v>46001.46237803435</v>
+        <v>46009.22343447226</v>
       </c>
       <c r="J8">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="K8">
         <v>6</v>
@@ -856,10 +856,10 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N8">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -888,7 +888,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="2">
-        <v>46001.46237803435</v>
+        <v>46009.22343447226</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -917,25 +917,25 @@
         <v>36</v>
       </c>
       <c r="D10">
+        <v>971</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>964</v>
+      </c>
+      <c r="G10">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>964</v>
+      </c>
+      <c r="I10" s="2">
+        <v>46009.22343447226</v>
+      </c>
+      <c r="J10">
         <v>984</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>973</v>
-      </c>
-      <c r="G10">
-        <v>22</v>
-      </c>
-      <c r="H10">
-        <v>973</v>
-      </c>
-      <c r="I10" s="2">
-        <v>46001.46237803435</v>
-      </c>
-      <c r="J10">
-        <v>993</v>
       </c>
       <c r="K10">
         <v>27</v>
@@ -947,7 +947,7 @@
         <v>7</v>
       </c>
       <c r="N10">
-        <v>973</v>
+        <v>964</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -961,25 +961,25 @@
         <v>37</v>
       </c>
       <c r="D11">
-        <v>1133</v>
+        <v>1088</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1082</v>
       </c>
       <c r="G11">
-        <v>2266</v>
+        <v>12</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1082</v>
       </c>
       <c r="I11" s="2">
-        <v>46001.46237803435</v>
+        <v>46009.22343448379</v>
       </c>
       <c r="J11">
-        <v>4</v>
+        <v>1091</v>
       </c>
       <c r="K11">
         <v>25</v>
@@ -988,10 +988,10 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1020,7 +1020,7 @@
         <v>508</v>
       </c>
       <c r="I12" s="2">
-        <v>46001.46237803435</v>
+        <v>46009.22343448379</v>
       </c>
       <c r="J12">
         <v>507</v>
@@ -1064,7 +1064,7 @@
         <v>106</v>
       </c>
       <c r="I13" s="2">
-        <v>46001.46237803435</v>
+        <v>46009.22343447226</v>
       </c>
       <c r="J13">
         <v>106</v>
@@ -1122,25 +1122,25 @@
         <v>41</v>
       </c>
       <c r="D15">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
       <c r="H15">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="I15" s="2">
-        <v>46001.46237803435</v>
+        <v>46009.22343447226</v>
       </c>
       <c r="J15">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="K15">
         <v>4</v>
@@ -1152,7 +1152,7 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1160,22 +1160,22 @@
         <v>42</v>
       </c>
       <c r="D16">
-        <v>11075</v>
+        <v>10772</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16">
-        <v>8942</v>
+        <v>10305</v>
       </c>
       <c r="G16">
-        <v>4240</v>
+        <v>210</v>
       </c>
       <c r="H16">
-        <v>8942</v>
+        <v>10305</v>
       </c>
       <c r="J16">
-        <v>9055</v>
+        <v>10425</v>
       </c>
       <c r="K16">
         <v>373</v>
@@ -1184,10 +1184,10 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <v>280</v>
+        <v>253</v>
       </c>
       <c r="N16">
-        <v>8942</v>
+        <v>10305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update code backend and frontend to fetch 12 months+
</commit_message>
<xml_diff>
--- a/backend/uploads/currentinventory_1_uk_december2025.xlsx
+++ b/backend/uploads/currentinventory_1_uk_december2025.xlsx
@@ -542,16 +542,16 @@
         <v>46004.27260633002</v>
       </c>
       <c r="J2" t="n">
-        <v>5059</v>
+        <v>5118</v>
       </c>
       <c r="K2" t="n">
-        <v>252</v>
+        <v>296</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="N2" t="n">
         <v>4973</v>
@@ -590,16 +590,16 @@
         <v>46004.27260633002</v>
       </c>
       <c r="J3" t="n">
-        <v>862</v>
+        <v>871</v>
       </c>
       <c r="K3" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="N3" t="n">
         <v>877</v>
@@ -638,16 +638,16 @@
         <v>46004.27260633002</v>
       </c>
       <c r="J4" t="n">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="K4" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N4" t="n">
         <v>578</v>
@@ -734,10 +734,10 @@
         <v>46004.27260633002</v>
       </c>
       <c r="J6" t="n">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="K6" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
@@ -782,16 +782,16 @@
         <v>46004.27260633002</v>
       </c>
       <c r="J7" t="n">
-        <v>966</v>
+        <v>984</v>
       </c>
       <c r="K7" t="n">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N7" t="n">
         <v>927</v>
@@ -926,10 +926,10 @@
         <v>46004.27260633002</v>
       </c>
       <c r="J10" t="n">
-        <v>994</v>
+        <v>999</v>
       </c>
       <c r="K10" t="n">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
@@ -974,16 +974,16 @@
         <v>46004.27260633002</v>
       </c>
       <c r="J11" t="n">
-        <v>1113</v>
+        <v>1129</v>
       </c>
       <c r="K11" t="n">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="N11" t="n">
         <v>1106</v>
@@ -1196,16 +1196,16 @@
       </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="n">
-        <v>11001</v>
+        <v>11115</v>
       </c>
       <c r="K16" t="n">
-        <v>439</v>
+        <v>527</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
       </c>
       <c r="M16" t="n">
-        <v>302</v>
+        <v>276</v>
       </c>
       <c r="N16" t="n">
         <v>10864</v>

</xml_diff>

<commit_message>
cashflow complete code update backend and forntend
</commit_message>
<xml_diff>
--- a/backend/uploads/currentinventory_1_uk_december2025.xlsx
+++ b/backend/uploads/currentinventory_1_uk_december2025.xlsx
@@ -612,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>4588</v>
+        <v>4576</v>
       </c>
       <c r="K2">
         <v>11</v>
@@ -630,13 +630,13 @@
         <v>4613</v>
       </c>
       <c r="P2">
-        <v>4122</v>
+        <v>3853</v>
       </c>
       <c r="Q2">
-        <v>511.68</v>
+        <v>510.29</v>
       </c>
       <c r="R2">
-        <v>5120</v>
+        <v>5108</v>
       </c>
       <c r="S2">
         <v>543</v>
@@ -648,7 +648,7 @@
         <v>11</v>
       </c>
       <c r="V2">
-        <v>4588</v>
+        <v>4576</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -683,10 +683,10 @@
         <v>454</v>
       </c>
       <c r="P3">
-        <v>38350</v>
+        <v>26962</v>
       </c>
       <c r="Q3">
-        <v>71.45</v>
+        <v>71.26000000000001</v>
       </c>
       <c r="R3">
         <v>910</v>
@@ -736,16 +736,16 @@
         <v>232</v>
       </c>
       <c r="P4">
-        <v>35611</v>
+        <v>21152</v>
       </c>
       <c r="Q4">
         <v>31.45</v>
       </c>
       <c r="R4">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="S4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T4">
         <v>0</v>
@@ -789,7 +789,7 @@
         <v>59</v>
       </c>
       <c r="P5">
-        <v>143228</v>
+        <v>144550</v>
       </c>
       <c r="Q5">
         <v>8.029999999999999</v>
@@ -824,7 +824,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -842,16 +842,16 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>27236</v>
+        <v>38454</v>
       </c>
       <c r="Q6">
-        <v>32.43</v>
+        <v>32.3</v>
       </c>
       <c r="R6">
         <v>305</v>
       </c>
       <c r="S6">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -860,7 +860,7 @@
         <v>3</v>
       </c>
       <c r="V6">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -877,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="K7">
         <v>43</v>
@@ -895,16 +895,16 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>10367</v>
+        <v>12903</v>
       </c>
       <c r="Q7">
-        <v>92.95</v>
+        <v>92.45999999999999</v>
       </c>
       <c r="R7">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="S7">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="T7">
         <v>0</v>
@@ -913,7 +913,7 @@
         <v>2</v>
       </c>
       <c r="V7">
-        <v>793</v>
+        <v>790</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -948,10 +948,10 @@
         <v>313</v>
       </c>
       <c r="P8">
-        <v>151489</v>
+        <v>152271</v>
       </c>
       <c r="Q8">
-        <v>35.75</v>
+        <v>35.74</v>
       </c>
       <c r="R8">
         <v>338</v>
@@ -1033,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>4122</v>
+        <v>3853</v>
       </c>
       <c r="Q10">
         <v>113.04</v>
@@ -1086,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <v>4122</v>
+        <v>3853</v>
       </c>
       <c r="Q11">
         <v>98.22</v>
@@ -1142,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>61.92</v>
+        <v>61.91</v>
       </c>
       <c r="R12">
         <v>511</v>
@@ -1192,10 +1192,10 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <v>124829</v>
+        <v>140624</v>
       </c>
       <c r="Q13">
-        <v>20.1</v>
+        <v>20.08</v>
       </c>
       <c r="R13">
         <v>105</v>
@@ -1277,10 +1277,10 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>97001</v>
+        <v>103756</v>
       </c>
       <c r="Q15">
-        <v>42.55</v>
+        <v>42.53</v>
       </c>
       <c r="R15">
         <v>172</v>
@@ -1306,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>9854</v>
+        <v>9838</v>
       </c>
       <c r="K16">
         <v>486</v>
@@ -1324,16 +1324,16 @@
         <v>5671</v>
       </c>
       <c r="P16">
-        <v>640477</v>
+        <v>652231</v>
       </c>
       <c r="Q16">
-        <v>1119.57</v>
+        <v>1117.31</v>
       </c>
       <c r="R16">
-        <v>10926</v>
+        <v>10913</v>
       </c>
       <c r="S16">
-        <v>1097</v>
+        <v>1100</v>
       </c>
       <c r="T16">
         <v>0</v>
@@ -1342,7 +1342,7 @@
         <v>25</v>
       </c>
       <c r="V16">
-        <v>9854</v>
+        <v>9838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>